<commit_message>
add files to the import dialog
</commit_message>
<xml_diff>
--- a/src/static/company_strctuer.xlsx
+++ b/src/static/company_strctuer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>First Name</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Company Street</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>string</t>
@@ -204,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -223,9 +220,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -553,45 +547,44 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="29.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="40.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="15" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="15" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="12" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="12" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="12" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="12" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="12" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="12" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="12" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="12" width="36.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="12" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="15" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="12" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="12" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="12" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="12" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="12" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="12" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="12" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="27.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="29.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="40.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="14" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="14" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="11" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="11" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="11" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="11" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="11" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="11" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="11" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="11" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="11" width="36.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="11" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="14" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="11" width="34.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="11" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="11" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="11" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="11" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="11" width="26.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -691,108 +684,102 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="7" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="Z2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="AB2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG2" s="7" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>